<commit_message>
Adding retries to create_3d_preview() to make it more stable
</commit_message>
<xml_diff>
--- a/STL_Checklist_Structured.xlsx
+++ b/STL_Checklist_Structured.xlsx
@@ -17,7 +17,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,10 +27,6 @@
     </font>
     <font>
       <b val="1"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <color rgb="00FF0000"/>
     </font>
   </fonts>
   <fills count="2">
@@ -53,9 +49,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1814,17 +1809,42 @@
     <from>
       <col>1</col>
       <colOff>0</colOff>
+      <row>98</row>
+      <rowOff>0</rowOff>
+    </from>
+    <ext cx="1905000" cy="1905000"/>
+    <pic>
+      <nvPicPr>
+        <cNvPr id="68" name="Image 68" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId68"/>
+        <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:fillRect/>
+        </a:stretch>
+      </blipFill>
+      <spPr>
+        <a:prstGeom xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" prst="rect"/>
+      </spPr>
+    </pic>
+    <clientData/>
+  </oneCellAnchor>
+  <oneCellAnchor>
+    <from>
+      <col>1</col>
+      <colOff>0</colOff>
       <row>101</row>
       <rowOff>0</rowOff>
     </from>
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="68" name="Image 68" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId68"/>
+        <cNvPr id="69" name="Image 69" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId69"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1845,11 +1865,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="69" name="Image 69" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId69"/>
+        <cNvPr id="70" name="Image 70" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId70"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1870,11 +1890,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="70" name="Image 70" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId70"/>
+        <cNvPr id="71" name="Image 71" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId71"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1895,11 +1915,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="71" name="Image 71" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId71"/>
+        <cNvPr id="72" name="Image 72" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId72"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1920,11 +1940,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="72" name="Image 72" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId72"/>
+        <cNvPr id="73" name="Image 73" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId73"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1945,11 +1965,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="73" name="Image 73" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId73"/>
+        <cNvPr id="74" name="Image 74" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId74"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1970,11 +1990,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="74" name="Image 74" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId74"/>
+        <cNvPr id="75" name="Image 75" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId75"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -1995,11 +2015,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="75" name="Image 75" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId75"/>
+        <cNvPr id="76" name="Image 76" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId76"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2020,11 +2040,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="76" name="Image 76" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId76"/>
+        <cNvPr id="77" name="Image 77" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId77"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2045,11 +2065,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="77" name="Image 77" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId77"/>
+        <cNvPr id="78" name="Image 78" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId78"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2070,11 +2090,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="78" name="Image 78" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId78"/>
+        <cNvPr id="79" name="Image 79" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId79"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2095,11 +2115,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="79" name="Image 79" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId79"/>
+        <cNvPr id="80" name="Image 80" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId80"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2120,11 +2140,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="80" name="Image 80" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId80"/>
+        <cNvPr id="81" name="Image 81" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId81"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2145,11 +2165,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="81" name="Image 81" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId81"/>
+        <cNvPr id="82" name="Image 82" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId82"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2170,11 +2190,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="82" name="Image 82" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId82"/>
+        <cNvPr id="83" name="Image 83" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId83"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2195,11 +2215,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="83" name="Image 83" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId83"/>
+        <cNvPr id="84" name="Image 84" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId84"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2220,11 +2240,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="84" name="Image 84" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId84"/>
+        <cNvPr id="85" name="Image 85" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId85"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2245,11 +2265,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="85" name="Image 85" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId85"/>
+        <cNvPr id="86" name="Image 86" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId86"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2270,11 +2290,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="86" name="Image 86" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId86"/>
+        <cNvPr id="87" name="Image 87" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId87"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2295,11 +2315,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="87" name="Image 87" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId87"/>
+        <cNvPr id="88" name="Image 88" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId88"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2320,11 +2340,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="88" name="Image 88" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId88"/>
+        <cNvPr id="89" name="Image 89" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId89"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2345,11 +2365,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="89" name="Image 89" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId89"/>
+        <cNvPr id="90" name="Image 90" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId90"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2370,11 +2390,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="90" name="Image 90" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId90"/>
+        <cNvPr id="91" name="Image 91" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId91"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2395,11 +2415,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="91" name="Image 91" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId91"/>
+        <cNvPr id="92" name="Image 92" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId92"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2420,11 +2440,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="92" name="Image 92" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId92"/>
+        <cNvPr id="93" name="Image 93" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId93"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2445,11 +2465,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="93" name="Image 93" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId93"/>
+        <cNvPr id="94" name="Image 94" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId94"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2470,11 +2490,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="94" name="Image 94" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId94"/>
+        <cNvPr id="95" name="Image 95" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId95"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2495,11 +2515,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="95" name="Image 95" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId95"/>
+        <cNvPr id="96" name="Image 96" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId96"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2520,11 +2540,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="96" name="Image 96" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId96"/>
+        <cNvPr id="97" name="Image 97" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId97"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2545,11 +2565,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="97" name="Image 97" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId97"/>
+        <cNvPr id="98" name="Image 98" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId98"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2570,11 +2590,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="98" name="Image 98" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId98"/>
+        <cNvPr id="99" name="Image 99" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId99"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2595,11 +2615,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="99" name="Image 99" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId99"/>
+        <cNvPr id="100" name="Image 100" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId100"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2620,11 +2640,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="100" name="Image 100" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId100"/>
+        <cNvPr id="101" name="Image 101" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId101"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2645,11 +2665,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="101" name="Image 101" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId101"/>
+        <cNvPr id="102" name="Image 102" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId102"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2670,11 +2690,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="102" name="Image 102" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId102"/>
+        <cNvPr id="103" name="Image 103" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId103"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2695,11 +2715,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="103" name="Image 103" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId103"/>
+        <cNvPr id="104" name="Image 104" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId104"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2720,11 +2740,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="104" name="Image 104" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId104"/>
+        <cNvPr id="105" name="Image 105" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId105"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2745,11 +2765,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="105" name="Image 105" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId105"/>
+        <cNvPr id="106" name="Image 106" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId106"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2770,11 +2790,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="106" name="Image 106" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId106"/>
+        <cNvPr id="107" name="Image 107" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId107"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2795,11 +2815,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="107" name="Image 107" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId107"/>
+        <cNvPr id="108" name="Image 108" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId108"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2820,11 +2840,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="108" name="Image 108" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId108"/>
+        <cNvPr id="109" name="Image 109" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId109"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2845,11 +2865,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="109" name="Image 109" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId109"/>
+        <cNvPr id="110" name="Image 110" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId110"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2870,11 +2890,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="110" name="Image 110" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId110"/>
+        <cNvPr id="111" name="Image 111" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId111"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2895,11 +2915,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="111" name="Image 111" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId111"/>
+        <cNvPr id="112" name="Image 112" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId112"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2920,11 +2940,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="112" name="Image 112" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId112"/>
+        <cNvPr id="113" name="Image 113" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId113"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2945,11 +2965,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="113" name="Image 113" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId113"/>
+        <cNvPr id="114" name="Image 114" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId114"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2970,11 +2990,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="114" name="Image 114" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId114"/>
+        <cNvPr id="115" name="Image 115" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId115"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -2995,11 +3015,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="115" name="Image 115" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId115"/>
+        <cNvPr id="116" name="Image 116" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId116"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3020,11 +3040,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="116" name="Image 116" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId116"/>
+        <cNvPr id="117" name="Image 117" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId117"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3045,11 +3065,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="117" name="Image 117" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId117"/>
+        <cNvPr id="118" name="Image 118" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId118"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3070,11 +3090,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="118" name="Image 118" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId118"/>
+        <cNvPr id="119" name="Image 119" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId119"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3095,11 +3115,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="119" name="Image 119" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId119"/>
+        <cNvPr id="120" name="Image 120" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId120"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3120,11 +3140,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="120" name="Image 120" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId120"/>
+        <cNvPr id="121" name="Image 121" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId121"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3145,11 +3165,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="121" name="Image 121" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId121"/>
+        <cNvPr id="122" name="Image 122" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId122"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3170,11 +3190,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="122" name="Image 122" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId122"/>
+        <cNvPr id="123" name="Image 123" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId123"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3195,11 +3215,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="123" name="Image 123" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId123"/>
+        <cNvPr id="124" name="Image 124" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId124"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3220,11 +3240,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="124" name="Image 124" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId124"/>
+        <cNvPr id="125" name="Image 125" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId125"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3245,11 +3265,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="125" name="Image 125" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId125"/>
+        <cNvPr id="126" name="Image 126" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId126"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3270,11 +3290,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="126" name="Image 126" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId126"/>
+        <cNvPr id="127" name="Image 127" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId127"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3295,11 +3315,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="127" name="Image 127" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId127"/>
+        <cNvPr id="128" name="Image 128" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId128"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3320,11 +3340,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="128" name="Image 128" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId128"/>
+        <cNvPr id="129" name="Image 129" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId129"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3345,11 +3365,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="129" name="Image 129" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId129"/>
+        <cNvPr id="130" name="Image 130" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId130"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3370,11 +3390,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="130" name="Image 130" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId130"/>
+        <cNvPr id="131" name="Image 131" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId131"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3395,11 +3415,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="131" name="Image 131" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId131"/>
+        <cNvPr id="132" name="Image 132" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId132"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3420,11 +3440,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="132" name="Image 132" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId132"/>
+        <cNvPr id="133" name="Image 133" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId133"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3445,11 +3465,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="133" name="Image 133" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId133"/>
+        <cNvPr id="134" name="Image 134" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId134"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3470,11 +3490,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="134" name="Image 134" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId134"/>
+        <cNvPr id="135" name="Image 135" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId135"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3495,11 +3515,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="135" name="Image 135" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId135"/>
+        <cNvPr id="136" name="Image 136" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId136"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3520,11 +3540,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="136" name="Image 136" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId136"/>
+        <cNvPr id="137" name="Image 137" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId137"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3545,11 +3565,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="137" name="Image 137" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId137"/>
+        <cNvPr id="138" name="Image 138" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId138"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3570,11 +3590,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="138" name="Image 138" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId138"/>
+        <cNvPr id="139" name="Image 139" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId139"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3595,11 +3615,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="139" name="Image 139" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId139"/>
+        <cNvPr id="140" name="Image 140" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId140"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3620,11 +3640,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="140" name="Image 140" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId140"/>
+        <cNvPr id="141" name="Image 141" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId141"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3645,11 +3665,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="141" name="Image 141" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId141"/>
+        <cNvPr id="142" name="Image 142" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId142"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3670,11 +3690,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="142" name="Image 142" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId142"/>
+        <cNvPr id="143" name="Image 143" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId143"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3695,11 +3715,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="143" name="Image 143" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId143"/>
+        <cNvPr id="144" name="Image 144" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId144"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3720,11 +3740,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="144" name="Image 144" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId144"/>
+        <cNvPr id="145" name="Image 145" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId145"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3745,11 +3765,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="145" name="Image 145" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId145"/>
+        <cNvPr id="146" name="Image 146" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId146"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3770,11 +3790,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="146" name="Image 146" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId146"/>
+        <cNvPr id="147" name="Image 147" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId147"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3795,11 +3815,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="147" name="Image 147" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId147"/>
+        <cNvPr id="148" name="Image 148" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId148"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3820,11 +3840,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="148" name="Image 148" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId148"/>
+        <cNvPr id="149" name="Image 149" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId149"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -3845,11 +3865,11 @@
     <ext cx="1905000" cy="1905000"/>
     <pic>
       <nvPicPr>
-        <cNvPr id="149" name="Image 149" descr="Picture"/>
-        <cNvPicPr/>
-      </nvPicPr>
-      <blipFill>
-        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId149"/>
+        <cNvPr id="150" name="Image 150" descr="Picture"/>
+        <cNvPicPr/>
+      </nvPicPr>
+      <blipFill>
+        <a:blip xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" cstate="print" r:embed="rId150"/>
         <a:stretch xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
           <a:fillRect/>
         </a:stretch>
@@ -4152,7 +4172,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D213"/>
+  <dimension ref="A1:D211"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4169,53 +4189,59 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Warning: The following STL files failed to generate a preview:</t>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Preview</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Checked and Available</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Not Needed</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Panel_Mounting/z_belt_cover_b_x2.stl</t>
-        </is>
-      </c>
+      <c r="A2" t="inlineStr"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Filename</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="inlineStr">
-        <is>
-          <t>Preview</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="inlineStr">
-        <is>
-          <t>Checked and Available</t>
-        </is>
-      </c>
-      <c r="D3" s="2" t="inlineStr">
-        <is>
-          <t>Not Needed</t>
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Electronics_Bay\Controller_Mounts</t>
         </is>
       </c>
     </row>
     <row r="4" ht="150" customHeight="1">
-      <c r="A4" t="inlineStr"/>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>BIGDIPPER_bracket_set.stl</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
+      <c r="D4" t="inlineStr"/>
     </row>
     <row r="5" ht="150" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Electronics_Bay\Controller_Mounts</t>
-        </is>
-      </c>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>BTT_MOT_EXP_bracket.stl</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
     </row>
     <row r="6" ht="150" customHeight="1">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BIGDIPPER_bracket_set.stl</t>
+          <t>Duet2_Duet3Mini5_bracket_set.stl</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
@@ -4225,7 +4251,7 @@
     <row r="7" ht="150" customHeight="1">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BTT_MOT_EXP_bracket.stl</t>
+          <t>GTR_bracket_set.stl</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
@@ -4235,7 +4261,7 @@
     <row r="8" ht="150" customHeight="1">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Duet2_Duet3Mini5_bracket_set.stl</t>
+          <t>Octopus_bracket_set.stl</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
@@ -4245,7 +4271,7 @@
     <row r="9" ht="150" customHeight="1">
       <c r="A9" t="inlineStr">
         <is>
-          <t>GTR_bracket_set.stl</t>
+          <t>S6_bracket_set.stl</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
@@ -4255,7 +4281,7 @@
     <row r="10" ht="150" customHeight="1">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Octopus_bracket_set.stl</t>
+          <t>SKR_bracket_inline_set.stl</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
@@ -4265,7 +4291,7 @@
     <row r="11" ht="150" customHeight="1">
       <c r="A11" t="inlineStr">
         <is>
-          <t>S6_bracket_set.stl</t>
+          <t>SKR_Pro_bracket_set.stl</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
@@ -4275,7 +4301,7 @@
     <row r="12" ht="150" customHeight="1">
       <c r="A12" t="inlineStr">
         <is>
-          <t>SKR_bracket_inline_set.stl</t>
+          <t>Spider_bracket_set.stl</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
@@ -4283,89 +4309,89 @@
       <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>SKR_Pro_bracket_set.stl</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
+      <c r="A13" t="inlineStr"/>
     </row>
     <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>Spider_bracket_set.stl</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Electronics_Bay</t>
+        </is>
+      </c>
     </row>
     <row r="15" ht="150" customHeight="1">
-      <c r="A15" t="inlineStr"/>
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>lrs_200_psu_bracket_x2.stl</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
+      <c r="A16" t="inlineStr"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Electronics_Bay\Other_PS_Mounts</t>
+        </is>
+      </c>
+    </row>
+    <row r="18" ht="150" customHeight="1">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>UHP_200_Mount_x2.stl</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
+    </row>
+    <row r="19" ht="150" customHeight="1">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>UHP_350_Mount_x2.stl</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="1" t="inlineStr">
         <is>
           <t>Folder: Electronics_Bay</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>lrs_200_psu_bracket_x2.stl</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
-    </row>
-    <row r="18" ht="150" customHeight="1">
-      <c r="A18" t="inlineStr"/>
-    </row>
-    <row r="19" ht="150" customHeight="1">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Electronics_Bay\Other_PS_Mounts</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
-        <is>
-          <t>UHP_200_Mount_x2.stl</t>
-        </is>
-      </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>UHP_350_Mount_x2.stl</t>
-        </is>
-      </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
-    </row>
     <row r="22" ht="150" customHeight="1">
-      <c r="A22" t="inlineStr"/>
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>pcb_din_clip_x3.stl</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr"/>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
     </row>
     <row r="23" ht="150" customHeight="1">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Electronics_Bay</t>
-        </is>
-      </c>
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>PSU_stabilizer_50mm.stl</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr"/>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
     </row>
     <row r="24" ht="150" customHeight="1">
       <c r="A24" t="inlineStr">
         <is>
-          <t>pcb_din_clip_x3.stl</t>
+          <t>raspberrypi_bracket.stl</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -4375,7 +4401,7 @@
     <row r="25" ht="150" customHeight="1">
       <c r="A25" t="inlineStr">
         <is>
-          <t>PSU_stabilizer_50mm.stl</t>
+          <t>rs25_psu_bracket.stl</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -4385,7 +4411,7 @@
     <row r="26" ht="150" customHeight="1">
       <c r="A26" t="inlineStr">
         <is>
-          <t>raspberrypi_bracket.stl</t>
+          <t>wago_221-415_mount_3by5.stl</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -4393,39 +4419,39 @@
       <c r="D26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>rs25_psu_bracket.stl</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr"/>
-      <c r="C27" t="inlineStr"/>
-      <c r="D27" t="inlineStr"/>
+      <c r="A27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>wago_221-415_mount_3by5.stl</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr"/>
-      <c r="C28" t="inlineStr"/>
-      <c r="D28" t="inlineStr"/>
+      <c r="A28" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Exhaust_Filter</t>
+        </is>
+      </c>
     </row>
     <row r="29" ht="150" customHeight="1">
-      <c r="A29" t="inlineStr"/>
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>[a]_exhaust_fan_grill.stl</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr"/>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
     </row>
     <row r="30" ht="150" customHeight="1">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Exhaust_Filter</t>
-        </is>
-      </c>
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>[a]_exhaust_filter_mount_x2.stl</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr"/>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
     </row>
     <row r="31" ht="150" customHeight="1">
       <c r="A31" t="inlineStr">
         <is>
-          <t>[a]_exhaust_fan_grill.stl</t>
+          <t>[a]_filter_access_cover.stl</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -4435,7 +4461,7 @@
     <row r="32" ht="150" customHeight="1">
       <c r="A32" t="inlineStr">
         <is>
-          <t>[a]_exhaust_filter_mount_x2.stl</t>
+          <t>exhaust_filter_grill.stl</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -4445,7 +4471,7 @@
     <row r="33" ht="150" customHeight="1">
       <c r="A33" t="inlineStr">
         <is>
-          <t>[a]_filter_access_cover.stl</t>
+          <t>exhaust_filter_housing.stl</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -4453,69 +4479,69 @@
       <c r="D33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>exhaust_filter_grill.stl</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr"/>
-      <c r="C34" t="inlineStr"/>
-      <c r="D34" t="inlineStr"/>
+      <c r="A34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>exhaust_filter_housing.stl</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr"/>
-      <c r="C35" t="inlineStr"/>
-      <c r="D35" t="inlineStr"/>
+      <c r="A35" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry</t>
+        </is>
+      </c>
     </row>
     <row r="36" ht="150" customHeight="1">
-      <c r="A36" t="inlineStr"/>
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>[a]_z_belt_clip_lower_x4.stl</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr"/>
+      <c r="C36" t="inlineStr"/>
+      <c r="D36" t="inlineStr"/>
     </row>
     <row r="37" ht="150" customHeight="1">
-      <c r="A37" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry</t>
-        </is>
-      </c>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>[a]_z_belt_clip_upper_x4.stl</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr"/>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>[a]_z_belt_clip_lower_x4.stl</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr"/>
-      <c r="C38" t="inlineStr"/>
-      <c r="D38" t="inlineStr"/>
+      <c r="A38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>[a]_z_belt_clip_upper_x4.stl</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr"/>
-      <c r="C39" t="inlineStr"/>
-      <c r="D39" t="inlineStr"/>
+      <c r="A39" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry\AB_Drive_Units</t>
+        </is>
+      </c>
     </row>
     <row r="40" ht="150" customHeight="1">
-      <c r="A40" t="inlineStr"/>
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>[a]_cable_cover.stl</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr"/>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
     </row>
     <row r="41" ht="150" customHeight="1">
-      <c r="A41" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry\AB_Drive_Units</t>
-        </is>
-      </c>
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>[a]_z_chain_retainer_bracket_x2.stl</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr"/>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
     </row>
     <row r="42" ht="150" customHeight="1">
       <c r="A42" t="inlineStr">
         <is>
-          <t>[a]_cable_cover.stl</t>
+          <t>a_drive_frame_lower.stl</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -4525,7 +4551,7 @@
     <row r="43" ht="150" customHeight="1">
       <c r="A43" t="inlineStr">
         <is>
-          <t>[a]_z_chain_retainer_bracket_x2.stl</t>
+          <t>a_drive_frame_upper.stl</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -4535,7 +4561,7 @@
     <row r="44" ht="150" customHeight="1">
       <c r="A44" t="inlineStr">
         <is>
-          <t>a_drive_frame_lower.stl</t>
+          <t>b_drive_frame_lower.stl</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -4545,7 +4571,7 @@
     <row r="45" ht="150" customHeight="1">
       <c r="A45" t="inlineStr">
         <is>
-          <t>a_drive_frame_upper.stl</t>
+          <t>b_drive_frame_upper.stl</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -4553,39 +4579,39 @@
       <c r="D45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>b_drive_frame_lower.stl</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr"/>
-      <c r="C46" t="inlineStr"/>
-      <c r="D46" t="inlineStr"/>
+      <c r="A46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>b_drive_frame_upper.stl</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr"/>
-      <c r="C47" t="inlineStr"/>
-      <c r="D47" t="inlineStr"/>
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry\Front_Idlers</t>
+        </is>
+      </c>
     </row>
     <row r="48" ht="150" customHeight="1">
-      <c r="A48" t="inlineStr"/>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>[a]_tensioner_left.stl</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr"/>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
     </row>
     <row r="49" ht="150" customHeight="1">
-      <c r="A49" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry\Front_Idlers</t>
-        </is>
-      </c>
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>[a]_tensioner_right.stl</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr"/>
+      <c r="C49" t="inlineStr"/>
+      <c r="D49" t="inlineStr"/>
     </row>
     <row r="50" ht="150" customHeight="1">
       <c r="A50" t="inlineStr">
         <is>
-          <t>[a]_tensioner_left.stl</t>
+          <t>front_idler_left_lower.stl</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -4595,7 +4621,7 @@
     <row r="51" ht="150" customHeight="1">
       <c r="A51" t="inlineStr">
         <is>
-          <t>[a]_tensioner_right.stl</t>
+          <t>front_idler_left_upper.stl</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -4605,7 +4631,7 @@
     <row r="52" ht="150" customHeight="1">
       <c r="A52" t="inlineStr">
         <is>
-          <t>front_idler_left_lower.stl</t>
+          <t>front_idler_right_lower.stl</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -4615,7 +4641,7 @@
     <row r="53" ht="150" customHeight="1">
       <c r="A53" t="inlineStr">
         <is>
-          <t>front_idler_left_upper.stl</t>
+          <t>front_idler_right_upper.stl</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -4623,39 +4649,39 @@
       <c r="D53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>front_idler_right_lower.stl</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr"/>
-      <c r="C54" t="inlineStr"/>
-      <c r="D54" t="inlineStr"/>
+      <c r="A54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>front_idler_right_upper.stl</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr"/>
-      <c r="C55" t="inlineStr"/>
-      <c r="D55" t="inlineStr"/>
+      <c r="A55" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry\X_Axis\X_Carriage</t>
+        </is>
+      </c>
     </row>
     <row r="56" ht="150" customHeight="1">
-      <c r="A56" t="inlineStr"/>
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>pinda_adapter.stl</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr"/>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
     </row>
     <row r="57" ht="150" customHeight="1">
-      <c r="A57" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry\X_Axis\X_Carriage</t>
-        </is>
-      </c>
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>probe_retainer_bracket.stl</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr"/>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
     </row>
     <row r="58" ht="150" customHeight="1">
       <c r="A58" t="inlineStr">
         <is>
-          <t>pinda_adapter.stl</t>
+          <t>probe_retainer_bracket_9mm.stl</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -4665,7 +4691,7 @@
     <row r="59" ht="150" customHeight="1">
       <c r="A59" t="inlineStr">
         <is>
-          <t>probe_retainer_bracket.stl</t>
+          <t>x_frame_V2TR_MGN12_left.stl</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -4675,7 +4701,7 @@
     <row r="60" ht="150" customHeight="1">
       <c r="A60" t="inlineStr">
         <is>
-          <t>probe_retainer_bracket_9mm.stl</t>
+          <t>x_frame_V2TR_MGN12_right.stl</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -4683,39 +4709,39 @@
       <c r="D60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>x_frame_V2TR_MGN12_left.stl</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr"/>
-      <c r="C61" t="inlineStr"/>
-      <c r="D61" t="inlineStr"/>
+      <c r="A61" t="inlineStr"/>
     </row>
     <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>x_frame_V2TR_MGN12_right.stl</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr"/>
-      <c r="C62" t="inlineStr"/>
-      <c r="D62" t="inlineStr"/>
+      <c r="A62" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry\X_Axis\XY_Joints</t>
+        </is>
+      </c>
     </row>
     <row r="63" ht="150" customHeight="1">
-      <c r="A63" t="inlineStr"/>
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>[a]_endstop_pod_D2F_switch.stl</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr"/>
+      <c r="C63" t="inlineStr"/>
+      <c r="D63" t="inlineStr"/>
     </row>
     <row r="64" ht="150" customHeight="1">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry\X_Axis\XY_Joints</t>
-        </is>
-      </c>
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>[a]_endstop_pod_hall_effect.stl</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr"/>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
     </row>
     <row r="65" ht="150" customHeight="1">
       <c r="A65" t="inlineStr">
         <is>
-          <t>[a]_endstop_pod_D2F_switch.stl</t>
+          <t>[a]_xy_joint_cable_bridge_2hole.stl</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
@@ -4725,7 +4751,7 @@
     <row r="66" ht="150" customHeight="1">
       <c r="A66" t="inlineStr">
         <is>
-          <t>[a]_endstop_pod_hall_effect.stl</t>
+          <t>[a]_xy_joint_cable_bridge_3hole.stl</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
@@ -4735,7 +4761,7 @@
     <row r="67" ht="150" customHeight="1">
       <c r="A67" t="inlineStr">
         <is>
-          <t>[a]_xy_joint_cable_bridge_2hole.stl</t>
+          <t>xy_joint_left_lower_MGN12.stl</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
@@ -4745,7 +4771,7 @@
     <row r="68" ht="150" customHeight="1">
       <c r="A68" t="inlineStr">
         <is>
-          <t>[a]_xy_joint_cable_bridge_3hole.stl</t>
+          <t>xy_joint_left_upper_MGN12.stl</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
@@ -4755,7 +4781,7 @@
     <row r="69" ht="150" customHeight="1">
       <c r="A69" t="inlineStr">
         <is>
-          <t>xy_joint_left_lower_MGN12.stl</t>
+          <t>xy_joint_right_lower_MGN12.stl</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
@@ -4765,7 +4791,7 @@
     <row r="70" ht="150" customHeight="1">
       <c r="A70" t="inlineStr">
         <is>
-          <t>xy_joint_left_upper_MGN12.stl</t>
+          <t>xy_joint_right_upper_MGN12.stl</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
@@ -4773,69 +4799,69 @@
       <c r="D70" t="inlineStr"/>
     </row>
     <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>xy_joint_right_lower_MGN12.stl</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr"/>
-      <c r="C71" t="inlineStr"/>
-      <c r="D71" t="inlineStr"/>
+      <c r="A71" t="inlineStr"/>
     </row>
     <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>xy_joint_right_upper_MGN12.stl</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr"/>
-      <c r="C72" t="inlineStr"/>
-      <c r="D72" t="inlineStr"/>
+      <c r="A72" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry</t>
+        </is>
+      </c>
     </row>
     <row r="73" ht="150" customHeight="1">
-      <c r="A73" t="inlineStr"/>
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>z_chain_bottom_anchor.stl</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr"/>
+      <c r="C73" t="inlineStr"/>
+      <c r="D73" t="inlineStr"/>
     </row>
     <row r="74" ht="150" customHeight="1">
-      <c r="A74" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry</t>
-        </is>
-      </c>
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>z_chain_guide.stl</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr"/>
+      <c r="C74" t="inlineStr"/>
+      <c r="D74" t="inlineStr"/>
     </row>
     <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>z_chain_bottom_anchor.stl</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr"/>
-      <c r="C75" t="inlineStr"/>
-      <c r="D75" t="inlineStr"/>
+      <c r="A75" t="inlineStr"/>
     </row>
     <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>z_chain_guide.stl</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr"/>
-      <c r="C76" t="inlineStr"/>
-      <c r="D76" t="inlineStr"/>
+      <c r="A76" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Gantry\Z_Joints</t>
+        </is>
+      </c>
     </row>
     <row r="77" ht="150" customHeight="1">
-      <c r="A77" t="inlineStr"/>
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>z_joint_lower_x4.stl</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr"/>
+      <c r="C77" t="inlineStr"/>
+      <c r="D77" t="inlineStr"/>
     </row>
     <row r="78" ht="150" customHeight="1">
-      <c r="A78" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Gantry\Z_Joints</t>
-        </is>
-      </c>
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>z_joint_upper_hall_effect.stl</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr"/>
+      <c r="C78" t="inlineStr"/>
+      <c r="D78" t="inlineStr"/>
     </row>
     <row r="79" ht="150" customHeight="1">
       <c r="A79" t="inlineStr">
         <is>
-          <t>z_joint_lower_x4.stl</t>
+          <t>z_joint_upper_x4.stl</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
@@ -4843,39 +4869,39 @@
       <c r="D79" t="inlineStr"/>
     </row>
     <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>z_joint_upper_hall_effect.stl</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr"/>
-      <c r="C80" t="inlineStr"/>
-      <c r="D80" t="inlineStr"/>
+      <c r="A80" t="inlineStr"/>
     </row>
     <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>z_joint_upper_x4.stl</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr"/>
-      <c r="C81" t="inlineStr"/>
-      <c r="D81" t="inlineStr"/>
+      <c r="A81" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Panel_Mounting</t>
+        </is>
+      </c>
     </row>
     <row r="82" ht="150" customHeight="1">
-      <c r="A82" t="inlineStr"/>
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>bottom_panel_clip_x4.stl</t>
+        </is>
+      </c>
+      <c r="B82" t="inlineStr"/>
+      <c r="C82" t="inlineStr"/>
+      <c r="D82" t="inlineStr"/>
     </row>
     <row r="83" ht="150" customHeight="1">
-      <c r="A83" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Panel_Mounting</t>
-        </is>
-      </c>
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>bottom_panel_hinge_x2.stl</t>
+        </is>
+      </c>
+      <c r="B83" t="inlineStr"/>
+      <c r="C83" t="inlineStr"/>
+      <c r="D83" t="inlineStr"/>
     </row>
     <row r="84" ht="150" customHeight="1">
       <c r="A84" t="inlineStr">
         <is>
-          <t>bottom_panel_clip_x4.stl</t>
+          <t>corner_panel_clip_4mm_x8.stl</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
@@ -4885,7 +4911,7 @@
     <row r="85" ht="150" customHeight="1">
       <c r="A85" t="inlineStr">
         <is>
-          <t>bottom_panel_hinge_x2.stl</t>
+          <t>corner_panel_clip_6mm_x8.stl</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
@@ -4895,7 +4921,7 @@
     <row r="86" ht="150" customHeight="1">
       <c r="A86" t="inlineStr">
         <is>
-          <t>corner_panel_clip_4mm_x8.stl</t>
+          <t>deck_support_3mm_x8.stl</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
@@ -4905,7 +4931,7 @@
     <row r="87" ht="150" customHeight="1">
       <c r="A87" t="inlineStr">
         <is>
-          <t>corner_panel_clip_6mm_x8.stl</t>
+          <t>deck_support_4mm_x8.stl</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
@@ -4913,39 +4939,39 @@
       <c r="D87" t="inlineStr"/>
     </row>
     <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>deck_support_3mm_x8.stl</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr"/>
-      <c r="C88" t="inlineStr"/>
-      <c r="D88" t="inlineStr"/>
+      <c r="A88" t="inlineStr"/>
     </row>
     <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>deck_support_4mm_x8.stl</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
-      <c r="D89" t="inlineStr"/>
+      <c r="A89" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Panel_Mounting\Front_Doors</t>
+        </is>
+      </c>
     </row>
     <row r="90" ht="150" customHeight="1">
-      <c r="A90" t="inlineStr"/>
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>door_hinge_x6.stl</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr"/>
+      <c r="C90" t="inlineStr"/>
+      <c r="D90" t="inlineStr"/>
     </row>
     <row r="91" ht="150" customHeight="1">
-      <c r="A91" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Panel_Mounting\Front_Doors</t>
-        </is>
-      </c>
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>handle_a_x2.stl</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr"/>
+      <c r="C91" t="inlineStr"/>
+      <c r="D91" t="inlineStr"/>
     </row>
     <row r="92" ht="150" customHeight="1">
       <c r="A92" t="inlineStr">
         <is>
-          <t>door_hinge_x6.stl</t>
+          <t>handle_b_x2.stl</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
@@ -4955,7 +4981,7 @@
     <row r="93" ht="150" customHeight="1">
       <c r="A93" t="inlineStr">
         <is>
-          <t>handle_a_x2.stl</t>
+          <t>latch_x2.stl</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
@@ -4963,49 +4989,49 @@
       <c r="D93" t="inlineStr"/>
     </row>
     <row r="94">
-      <c r="A94" t="inlineStr">
-        <is>
-          <t>handle_b_x2.stl</t>
-        </is>
-      </c>
-      <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
-      <c r="D94" t="inlineStr"/>
+      <c r="A94" t="inlineStr"/>
     </row>
     <row r="95">
-      <c r="A95" t="inlineStr">
-        <is>
-          <t>latch_x2.stl</t>
-        </is>
-      </c>
-      <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
-      <c r="D95" t="inlineStr"/>
+      <c r="A95" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Panel_Mounting</t>
+        </is>
+      </c>
     </row>
     <row r="96" ht="150" customHeight="1">
-      <c r="A96" t="inlineStr"/>
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>midspan_panel_clip_4mm_x7.stl</t>
+        </is>
+      </c>
+      <c r="B96" t="inlineStr"/>
+      <c r="C96" t="inlineStr"/>
+      <c r="D96" t="inlineStr"/>
     </row>
     <row r="97" ht="150" customHeight="1">
-      <c r="A97" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Panel_Mounting</t>
-        </is>
-      </c>
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>midspan_panel_clip_6mm_x8.stl</t>
+        </is>
+      </c>
+      <c r="B97" t="inlineStr"/>
+      <c r="C97" t="inlineStr"/>
+      <c r="D97" t="inlineStr"/>
     </row>
     <row r="98" ht="150" customHeight="1">
       <c r="A98" t="inlineStr">
         <is>
-          <t>midspan_panel_clip_4mm_x7.stl</t>
+          <t>z_belt_cover_a_x2.stl</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
       <c r="C98" t="inlineStr"/>
       <c r="D98" t="inlineStr"/>
     </row>
-    <row r="99">
+    <row r="99" ht="150" customHeight="1">
       <c r="A99" t="inlineStr">
         <is>
-          <t>midspan_panel_clip_6mm_x8.stl</t>
+          <t>z_belt_cover_b_x2.stl</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
@@ -5013,43 +5039,39 @@
       <c r="D99" t="inlineStr"/>
     </row>
     <row r="100">
-      <c r="A100" t="inlineStr">
-        <is>
-          <t>z_belt_cover_a_x2.stl</t>
-        </is>
-      </c>
-      <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
-      <c r="D100" t="inlineStr"/>
+      <c r="A100" t="inlineStr"/>
     </row>
     <row r="101">
-      <c r="A101" t="inlineStr">
-        <is>
-          <t>z_belt_cover_b_x2.stl</t>
-        </is>
-      </c>
-      <c r="B101" t="inlineStr">
-        <is>
-          <t>Preview Missing</t>
-        </is>
-      </c>
-      <c r="C101" t="inlineStr"/>
-      <c r="D101" t="inlineStr"/>
+      <c r="A101" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Skirts\250</t>
+        </is>
+      </c>
     </row>
     <row r="102" ht="150" customHeight="1">
-      <c r="A102" t="inlineStr"/>
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>front_skirt_a_250.stl</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr"/>
+      <c r="C102" t="inlineStr"/>
+      <c r="D102" t="inlineStr"/>
     </row>
     <row r="103" ht="150" customHeight="1">
-      <c r="A103" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Skirts\250</t>
-        </is>
-      </c>
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>front_skirt_b_250.stl</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr"/>
+      <c r="C103" t="inlineStr"/>
+      <c r="D103" t="inlineStr"/>
     </row>
     <row r="104" ht="150" customHeight="1">
       <c r="A104" t="inlineStr">
         <is>
-          <t>front_skirt_a_250.stl</t>
+          <t>rear_center_skirt_250.stl</t>
         </is>
       </c>
       <c r="B104" t="inlineStr"/>
@@ -5059,7 +5081,7 @@
     <row r="105" ht="150" customHeight="1">
       <c r="A105" t="inlineStr">
         <is>
-          <t>front_skirt_b_250.stl</t>
+          <t>side_skirt_a_250_x2.stl</t>
         </is>
       </c>
       <c r="B105" t="inlineStr"/>
@@ -5069,7 +5091,7 @@
     <row r="106" ht="150" customHeight="1">
       <c r="A106" t="inlineStr">
         <is>
-          <t>rear_center_skirt_250.stl</t>
+          <t>side_skirt_b_250_x2.stl</t>
         </is>
       </c>
       <c r="B106" t="inlineStr"/>
@@ -5077,39 +5099,39 @@
       <c r="D106" t="inlineStr"/>
     </row>
     <row r="107">
-      <c r="A107" t="inlineStr">
-        <is>
-          <t>side_skirt_a_250_x2.stl</t>
-        </is>
-      </c>
-      <c r="B107" t="inlineStr"/>
-      <c r="C107" t="inlineStr"/>
-      <c r="D107" t="inlineStr"/>
+      <c r="A107" t="inlineStr"/>
     </row>
     <row r="108">
-      <c r="A108" t="inlineStr">
-        <is>
-          <t>side_skirt_b_250_x2.stl</t>
-        </is>
-      </c>
-      <c r="B108" t="inlineStr"/>
-      <c r="C108" t="inlineStr"/>
-      <c r="D108" t="inlineStr"/>
+      <c r="A108" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Skirts\300</t>
+        </is>
+      </c>
     </row>
     <row r="109" ht="150" customHeight="1">
-      <c r="A109" t="inlineStr"/>
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>front_skirt_a_300.stl</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr"/>
+      <c r="D109" t="inlineStr"/>
     </row>
     <row r="110" ht="150" customHeight="1">
-      <c r="A110" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Skirts\300</t>
-        </is>
-      </c>
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>front_skirt_b_300.stl</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr"/>
+      <c r="D110" t="inlineStr"/>
     </row>
     <row r="111" ht="150" customHeight="1">
       <c r="A111" t="inlineStr">
         <is>
-          <t>front_skirt_a_300.stl</t>
+          <t>rear_center_skirt_300.stl</t>
         </is>
       </c>
       <c r="B111" t="inlineStr"/>
@@ -5119,7 +5141,7 @@
     <row r="112" ht="150" customHeight="1">
       <c r="A112" t="inlineStr">
         <is>
-          <t>front_skirt_b_300.stl</t>
+          <t>side_skirt_a_300_x2.stl</t>
         </is>
       </c>
       <c r="B112" t="inlineStr"/>
@@ -5129,7 +5151,7 @@
     <row r="113" ht="150" customHeight="1">
       <c r="A113" t="inlineStr">
         <is>
-          <t>rear_center_skirt_300.stl</t>
+          <t>side_skirt_b_300_x2.stl</t>
         </is>
       </c>
       <c r="B113" t="inlineStr"/>
@@ -5137,39 +5159,39 @@
       <c r="D113" t="inlineStr"/>
     </row>
     <row r="114">
-      <c r="A114" t="inlineStr">
-        <is>
-          <t>side_skirt_a_300_x2.stl</t>
-        </is>
-      </c>
-      <c r="B114" t="inlineStr"/>
-      <c r="C114" t="inlineStr"/>
-      <c r="D114" t="inlineStr"/>
+      <c r="A114" t="inlineStr"/>
     </row>
     <row r="115">
-      <c r="A115" t="inlineStr">
-        <is>
-          <t>side_skirt_b_300_x2.stl</t>
-        </is>
-      </c>
-      <c r="B115" t="inlineStr"/>
-      <c r="C115" t="inlineStr"/>
-      <c r="D115" t="inlineStr"/>
+      <c r="A115" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Skirts\350</t>
+        </is>
+      </c>
     </row>
     <row r="116" ht="150" customHeight="1">
-      <c r="A116" t="inlineStr"/>
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>front_skirt_a_350.stl</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr"/>
+      <c r="D116" t="inlineStr"/>
     </row>
     <row r="117" ht="150" customHeight="1">
-      <c r="A117" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Skirts\350</t>
-        </is>
-      </c>
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>front_skirt_b_350.stl</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr"/>
+      <c r="D117" t="inlineStr"/>
     </row>
     <row r="118" ht="150" customHeight="1">
       <c r="A118" t="inlineStr">
         <is>
-          <t>front_skirt_a_350.stl</t>
+          <t>rear_center_skirt_350.stl</t>
         </is>
       </c>
       <c r="B118" t="inlineStr"/>
@@ -5179,7 +5201,7 @@
     <row r="119" ht="150" customHeight="1">
       <c r="A119" t="inlineStr">
         <is>
-          <t>front_skirt_b_350.stl</t>
+          <t>side_skirt_a_350_x2.stl</t>
         </is>
       </c>
       <c r="B119" t="inlineStr"/>
@@ -5189,7 +5211,7 @@
     <row r="120" ht="150" customHeight="1">
       <c r="A120" t="inlineStr">
         <is>
-          <t>rear_center_skirt_350.stl</t>
+          <t>side_skirt_b_350_x2.stl</t>
         </is>
       </c>
       <c r="B120" t="inlineStr"/>
@@ -5197,39 +5219,39 @@
       <c r="D120" t="inlineStr"/>
     </row>
     <row r="121">
-      <c r="A121" t="inlineStr">
-        <is>
-          <t>side_skirt_a_350_x2.stl</t>
-        </is>
-      </c>
-      <c r="B121" t="inlineStr"/>
-      <c r="C121" t="inlineStr"/>
-      <c r="D121" t="inlineStr"/>
+      <c r="A121" t="inlineStr"/>
     </row>
     <row r="122">
-      <c r="A122" t="inlineStr">
-        <is>
-          <t>side_skirt_b_350_x2.stl</t>
-        </is>
-      </c>
-      <c r="B122" t="inlineStr"/>
-      <c r="C122" t="inlineStr"/>
-      <c r="D122" t="inlineStr"/>
+      <c r="A122" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Skirts</t>
+        </is>
+      </c>
     </row>
     <row r="123" ht="150" customHeight="1">
-      <c r="A123" t="inlineStr"/>
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>[a]_belt_guard_a_x2.stl</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr"/>
+      <c r="C123" t="inlineStr"/>
+      <c r="D123" t="inlineStr"/>
     </row>
     <row r="124" ht="150" customHeight="1">
-      <c r="A124" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Skirts</t>
-        </is>
-      </c>
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>[a]_belt_guard_b_x2.stl</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr"/>
+      <c r="C124" t="inlineStr"/>
+      <c r="D124" t="inlineStr"/>
     </row>
     <row r="125" ht="150" customHeight="1">
       <c r="A125" t="inlineStr">
         <is>
-          <t>[a]_belt_guard_a_x2.stl</t>
+          <t>[a]_btt_knob_light_shield.stl</t>
         </is>
       </c>
       <c r="B125" t="inlineStr"/>
@@ -5239,7 +5261,7 @@
     <row r="126" ht="150" customHeight="1">
       <c r="A126" t="inlineStr">
         <is>
-          <t>[a]_belt_guard_b_x2.stl</t>
+          <t>[a]_fan_grill_a_x2.stl</t>
         </is>
       </c>
       <c r="B126" t="inlineStr"/>
@@ -5249,7 +5271,7 @@
     <row r="127" ht="150" customHeight="1">
       <c r="A127" t="inlineStr">
         <is>
-          <t>[a]_btt_knob_light_shield.stl</t>
+          <t>[a]_fan_grill_b_x2.stl</t>
         </is>
       </c>
       <c r="B127" t="inlineStr"/>
@@ -5259,7 +5281,7 @@
     <row r="128" ht="150" customHeight="1">
       <c r="A128" t="inlineStr">
         <is>
-          <t>[a]_fan_grill_a_x2.stl</t>
+          <t>[a]_fan_grill_open_optional_x2.stl</t>
         </is>
       </c>
       <c r="B128" t="inlineStr"/>
@@ -5269,7 +5291,7 @@
     <row r="129" ht="150" customHeight="1">
       <c r="A129" t="inlineStr">
         <is>
-          <t>[a]_fan_grill_b_x2.stl</t>
+          <t>[a]_fan_grill_retainer_x2.stl</t>
         </is>
       </c>
       <c r="B129" t="inlineStr"/>
@@ -5279,7 +5301,7 @@
     <row r="130" ht="150" customHeight="1">
       <c r="A130" t="inlineStr">
         <is>
-          <t>[a]_fan_grill_open_optional_x2.stl</t>
+          <t>[a]_keystone_blank_insert.stl</t>
         </is>
       </c>
       <c r="B130" t="inlineStr"/>
@@ -5289,7 +5311,7 @@
     <row r="131" ht="150" customHeight="1">
       <c r="A131" t="inlineStr">
         <is>
-          <t>[a]_fan_grill_retainer_x2.stl</t>
+          <t>[a]_mini12864_case_front_insert.stl</t>
         </is>
       </c>
       <c r="B131" t="inlineStr"/>
@@ -5299,7 +5321,7 @@
     <row r="132" ht="150" customHeight="1">
       <c r="A132" t="inlineStr">
         <is>
-          <t>[a]_keystone_blank_insert.stl</t>
+          <t>[a]_mini12864_case_hinge.stl</t>
         </is>
       </c>
       <c r="B132" t="inlineStr"/>
@@ -5309,7 +5331,7 @@
     <row r="133" ht="150" customHeight="1">
       <c r="A133" t="inlineStr">
         <is>
-          <t>[a]_mini12864_case_front_insert.stl</t>
+          <t>keystone_panel.stl</t>
         </is>
       </c>
       <c r="B133" t="inlineStr"/>
@@ -5319,7 +5341,7 @@
     <row r="134" ht="150" customHeight="1">
       <c r="A134" t="inlineStr">
         <is>
-          <t>[a]_mini12864_case_hinge.stl</t>
+          <t>mini12864_case_front.stl</t>
         </is>
       </c>
       <c r="B134" t="inlineStr"/>
@@ -5329,7 +5351,7 @@
     <row r="135" ht="150" customHeight="1">
       <c r="A135" t="inlineStr">
         <is>
-          <t>keystone_panel.stl</t>
+          <t>mini12864_case_rear.stl</t>
         </is>
       </c>
       <c r="B135" t="inlineStr"/>
@@ -5339,7 +5361,7 @@
     <row r="136" ht="150" customHeight="1">
       <c r="A136" t="inlineStr">
         <is>
-          <t>mini12864_case_front.stl</t>
+          <t>power_inlet_filtered.stl</t>
         </is>
       </c>
       <c r="B136" t="inlineStr"/>
@@ -5349,7 +5371,7 @@
     <row r="137" ht="150" customHeight="1">
       <c r="A137" t="inlineStr">
         <is>
-          <t>mini12864_case_rear.stl</t>
+          <t>power_inlet_IECGS_1.2mm.stl</t>
         </is>
       </c>
       <c r="B137" t="inlineStr"/>
@@ -5359,7 +5381,7 @@
     <row r="138" ht="150" customHeight="1">
       <c r="A138" t="inlineStr">
         <is>
-          <t>power_inlet_filtered.stl</t>
+          <t>power_inlet_IECGS_1mm.stl</t>
         </is>
       </c>
       <c r="B138" t="inlineStr"/>
@@ -5367,99 +5389,99 @@
       <c r="D138" t="inlineStr"/>
     </row>
     <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>power_inlet_IECGS_1.2mm.stl</t>
-        </is>
-      </c>
-      <c r="B139" t="inlineStr"/>
-      <c r="C139" t="inlineStr"/>
-      <c r="D139" t="inlineStr"/>
+      <c r="A139" t="inlineStr"/>
     </row>
     <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>power_inlet_IECGS_1mm.stl</t>
-        </is>
-      </c>
-      <c r="B140" t="inlineStr"/>
-      <c r="C140" t="inlineStr"/>
-      <c r="D140" t="inlineStr"/>
+      <c r="A140" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Spool_Management</t>
+        </is>
+      </c>
     </row>
     <row r="141" ht="150" customHeight="1">
-      <c r="A141" t="inlineStr"/>
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>bowden_retainer.stl</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr"/>
+      <c r="C141" t="inlineStr"/>
+      <c r="D141" t="inlineStr"/>
     </row>
     <row r="142" ht="150" customHeight="1">
-      <c r="A142" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Spool_Management</t>
-        </is>
-      </c>
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>spool_holder.stl</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr"/>
+      <c r="C142" t="inlineStr"/>
+      <c r="D142" t="inlineStr"/>
     </row>
     <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>bowden_retainer.stl</t>
-        </is>
-      </c>
-      <c r="B143" t="inlineStr"/>
-      <c r="C143" t="inlineStr"/>
-      <c r="D143" t="inlineStr"/>
+      <c r="A143" t="inlineStr"/>
     </row>
     <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>spool_holder.stl</t>
-        </is>
-      </c>
-      <c r="B144" t="inlineStr"/>
-      <c r="C144" t="inlineStr"/>
-      <c r="D144" t="inlineStr"/>
+      <c r="A144" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Superceded_Parts</t>
+        </is>
+      </c>
     </row>
     <row r="145" ht="150" customHeight="1">
-      <c r="A145" t="inlineStr"/>
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>[a]_stopgap_80T_hubbed_gear.stl</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr"/>
+      <c r="C145" t="inlineStr"/>
+      <c r="D145" t="inlineStr"/>
     </row>
     <row r="146" ht="150" customHeight="1">
-      <c r="A146" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Superceded_Parts</t>
-        </is>
-      </c>
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>[a]_z_tensioner_x4_6mm.stl</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr"/>
+      <c r="C146" t="inlineStr"/>
+      <c r="D146" t="inlineStr"/>
     </row>
     <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>[a]_stopgap_80T_hubbed_gear.stl</t>
-        </is>
-      </c>
-      <c r="B147" t="inlineStr"/>
-      <c r="C147" t="inlineStr"/>
-      <c r="D147" t="inlineStr"/>
+      <c r="A147" t="inlineStr"/>
     </row>
     <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>[a]_z_tensioner_x4_6mm.stl</t>
-        </is>
-      </c>
-      <c r="B148" t="inlineStr"/>
-      <c r="C148" t="inlineStr"/>
-      <c r="D148" t="inlineStr"/>
+      <c r="A148" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Superceded_Parts\Frame_Brackets</t>
+        </is>
+      </c>
     </row>
     <row r="149" ht="150" customHeight="1">
-      <c r="A149" t="inlineStr"/>
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>dual_ramps_bracket_frame.stl</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr"/>
+      <c r="C149" t="inlineStr"/>
+      <c r="D149" t="inlineStr"/>
     </row>
     <row r="150" ht="150" customHeight="1">
-      <c r="A150" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Superceded_Parts\Frame_Brackets</t>
-        </is>
-      </c>
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>duet_duex_bracket_frame_x2.stl</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr"/>
+      <c r="C150" t="inlineStr"/>
+      <c r="D150" t="inlineStr"/>
     </row>
     <row r="151" ht="150" customHeight="1">
       <c r="A151" t="inlineStr">
         <is>
-          <t>dual_ramps_bracket_frame.stl</t>
+          <t>lrs_bracket_frame.stl</t>
         </is>
       </c>
       <c r="B151" t="inlineStr"/>
@@ -5469,7 +5491,7 @@
     <row r="152" ht="150" customHeight="1">
       <c r="A152" t="inlineStr">
         <is>
-          <t>duet_duex_bracket_frame_x2.stl</t>
+          <t>mks_gen_1.4_bracket_frame_x2.stl</t>
         </is>
       </c>
       <c r="B152" t="inlineStr"/>
@@ -5479,7 +5501,7 @@
     <row r="153" ht="150" customHeight="1">
       <c r="A153" t="inlineStr">
         <is>
-          <t>lrs_bracket_frame.stl</t>
+          <t>mks_gen_L_bracket_frame_x2.stl</t>
         </is>
       </c>
       <c r="B153" t="inlineStr"/>
@@ -5489,7 +5511,7 @@
     <row r="154" ht="150" customHeight="1">
       <c r="A154" t="inlineStr">
         <is>
-          <t>mks_gen_1.4_bracket_frame_x2.stl</t>
+          <t>raspberry_pi_bracket.stl</t>
         </is>
       </c>
       <c r="B154" t="inlineStr"/>
@@ -5499,7 +5521,7 @@
     <row r="155" ht="150" customHeight="1">
       <c r="A155" t="inlineStr">
         <is>
-          <t>mks_gen_L_bracket_frame_x2.stl</t>
+          <t>rs_25_psu_bracket_frame.stl</t>
         </is>
       </c>
       <c r="B155" t="inlineStr"/>
@@ -5509,7 +5531,7 @@
     <row r="156" ht="150" customHeight="1">
       <c r="A156" t="inlineStr">
         <is>
-          <t>raspberry_pi_bracket.stl</t>
+          <t>rs_35_bracket_frame.stl</t>
         </is>
       </c>
       <c r="B156" t="inlineStr"/>
@@ -5519,7 +5541,7 @@
     <row r="157" ht="150" customHeight="1">
       <c r="A157" t="inlineStr">
         <is>
-          <t>rs_25_psu_bracket_frame.stl</t>
+          <t>skr_1.3_bracket_frame.stl</t>
         </is>
       </c>
       <c r="B157" t="inlineStr"/>
@@ -5529,7 +5551,7 @@
     <row r="158" ht="150" customHeight="1">
       <c r="A158" t="inlineStr">
         <is>
-          <t>rs_35_bracket_frame.stl</t>
+          <t>skr_mini_e3_bracket_frame.stl</t>
         </is>
       </c>
       <c r="B158" t="inlineStr"/>
@@ -5537,39 +5559,39 @@
       <c r="D158" t="inlineStr"/>
     </row>
     <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>skr_1.3_bracket_frame.stl</t>
-        </is>
-      </c>
-      <c r="B159" t="inlineStr"/>
-      <c r="C159" t="inlineStr"/>
-      <c r="D159" t="inlineStr"/>
+      <c r="A159" t="inlineStr"/>
     </row>
     <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>skr_mini_e3_bracket_frame.stl</t>
-        </is>
-      </c>
-      <c r="B160" t="inlineStr"/>
-      <c r="C160" t="inlineStr"/>
-      <c r="D160" t="inlineStr"/>
+      <c r="A160" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Superceded_Parts\MGN9_X</t>
+        </is>
+      </c>
     </row>
     <row r="161" ht="150" customHeight="1">
-      <c r="A161" t="inlineStr"/>
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>[a]_belt_clamp_MGN9_x2.stl</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr"/>
+      <c r="C161" t="inlineStr"/>
+      <c r="D161" t="inlineStr"/>
     </row>
     <row r="162" ht="150" customHeight="1">
-      <c r="A162" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Superceded_Parts\MGN9_X</t>
-        </is>
-      </c>
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>x_carriage_frame_left_MGN9.stl</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr"/>
+      <c r="C162" t="inlineStr"/>
+      <c r="D162" t="inlineStr"/>
     </row>
     <row r="163" ht="150" customHeight="1">
       <c r="A163" t="inlineStr">
         <is>
-          <t>[a]_belt_clamp_MGN9_x2.stl</t>
+          <t>x_carriage_frame_right_MGN9.stl</t>
         </is>
       </c>
       <c r="B163" t="inlineStr"/>
@@ -5579,7 +5601,7 @@
     <row r="164" ht="150" customHeight="1">
       <c r="A164" t="inlineStr">
         <is>
-          <t>x_carriage_frame_left_MGN9.stl</t>
+          <t>x_carriage_pivot_block_MGN9.stl</t>
         </is>
       </c>
       <c r="B164" t="inlineStr"/>
@@ -5589,7 +5611,7 @@
     <row r="165" ht="150" customHeight="1">
       <c r="A165" t="inlineStr">
         <is>
-          <t>x_carriage_frame_right_MGN9.stl</t>
+          <t>xy_joint_left_lower_MGN9.stl</t>
         </is>
       </c>
       <c r="B165" t="inlineStr"/>
@@ -5599,7 +5621,7 @@
     <row r="166" ht="150" customHeight="1">
       <c r="A166" t="inlineStr">
         <is>
-          <t>x_carriage_pivot_block_MGN9.stl</t>
+          <t>xy_joint_left_upper_MGN9.stl</t>
         </is>
       </c>
       <c r="B166" t="inlineStr"/>
@@ -5609,7 +5631,7 @@
     <row r="167" ht="150" customHeight="1">
       <c r="A167" t="inlineStr">
         <is>
-          <t>xy_joint_left_lower_MGN9.stl</t>
+          <t>xy_joint_right_lower_MGN9.stl</t>
         </is>
       </c>
       <c r="B167" t="inlineStr"/>
@@ -5619,7 +5641,7 @@
     <row r="168" ht="150" customHeight="1">
       <c r="A168" t="inlineStr">
         <is>
-          <t>xy_joint_left_upper_MGN9.stl</t>
+          <t>xy_joint_right_upper_MGN9.stl</t>
         </is>
       </c>
       <c r="B168" t="inlineStr"/>
@@ -5627,39 +5649,39 @@
       <c r="D168" t="inlineStr"/>
     </row>
     <row r="169">
-      <c r="A169" t="inlineStr">
-        <is>
-          <t>xy_joint_right_lower_MGN9.stl</t>
-        </is>
-      </c>
-      <c r="B169" t="inlineStr"/>
-      <c r="C169" t="inlineStr"/>
-      <c r="D169" t="inlineStr"/>
+      <c r="A169" t="inlineStr"/>
     </row>
     <row r="170">
-      <c r="A170" t="inlineStr">
-        <is>
-          <t>xy_joint_right_upper_MGN9.stl</t>
-        </is>
-      </c>
-      <c r="B170" t="inlineStr"/>
-      <c r="C170" t="inlineStr"/>
-      <c r="D170" t="inlineStr"/>
+      <c r="A170" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Superceded_Parts\ZipChain\XY</t>
+        </is>
+      </c>
     </row>
     <row r="171" ht="150" customHeight="1">
-      <c r="A171" t="inlineStr"/>
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>zipchain2_xy_end.stl</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr"/>
+      <c r="C171" t="inlineStr"/>
+      <c r="D171" t="inlineStr"/>
     </row>
     <row r="172" ht="150" customHeight="1">
-      <c r="A172" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Superceded_Parts\ZipChain\XY</t>
-        </is>
-      </c>
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>zipchain2_xy_link_a.stl</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr"/>
+      <c r="C172" t="inlineStr"/>
+      <c r="D172" t="inlineStr"/>
     </row>
     <row r="173" ht="150" customHeight="1">
       <c r="A173" t="inlineStr">
         <is>
-          <t>zipchain2_xy_end.stl</t>
+          <t>zipchain2_xy_link_b.stl</t>
         </is>
       </c>
       <c r="B173" t="inlineStr"/>
@@ -5667,39 +5689,39 @@
       <c r="D173" t="inlineStr"/>
     </row>
     <row r="174">
-      <c r="A174" t="inlineStr">
-        <is>
-          <t>zipchain2_xy_link_a.stl</t>
-        </is>
-      </c>
-      <c r="B174" t="inlineStr"/>
-      <c r="C174" t="inlineStr"/>
-      <c r="D174" t="inlineStr"/>
+      <c r="A174" t="inlineStr"/>
     </row>
     <row r="175">
-      <c r="A175" t="inlineStr">
-        <is>
-          <t>zipchain2_xy_link_b.stl</t>
-        </is>
-      </c>
-      <c r="B175" t="inlineStr"/>
-      <c r="C175" t="inlineStr"/>
-      <c r="D175" t="inlineStr"/>
+      <c r="A175" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Superceded_Parts\ZipChain\Z</t>
+        </is>
+      </c>
     </row>
     <row r="176" ht="150" customHeight="1">
-      <c r="A176" t="inlineStr"/>
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>zipchain2_z_end.stl</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr"/>
+      <c r="C176" t="inlineStr"/>
+      <c r="D176" t="inlineStr"/>
     </row>
     <row r="177" ht="150" customHeight="1">
-      <c r="A177" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Superceded_Parts\ZipChain\Z</t>
-        </is>
-      </c>
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>zipchain2_z_link_a.stl</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr"/>
+      <c r="C177" t="inlineStr"/>
+      <c r="D177" t="inlineStr"/>
     </row>
     <row r="178" ht="150" customHeight="1">
       <c r="A178" t="inlineStr">
         <is>
-          <t>zipchain2_z_end.stl</t>
+          <t>zipchain2_z_link_b.stl</t>
         </is>
       </c>
       <c r="B178" t="inlineStr"/>
@@ -5709,7 +5731,7 @@
     <row r="179" ht="150" customHeight="1">
       <c r="A179" t="inlineStr">
         <is>
-          <t>zipchain2_z_link_a.stl</t>
+          <t>zipchain2_z_link_b_locking.stl</t>
         </is>
       </c>
       <c r="B179" t="inlineStr"/>
@@ -5717,39 +5739,39 @@
       <c r="D179" t="inlineStr"/>
     </row>
     <row r="180">
-      <c r="A180" t="inlineStr">
-        <is>
-          <t>zipchain2_z_link_b.stl</t>
-        </is>
-      </c>
-      <c r="B180" t="inlineStr"/>
-      <c r="C180" t="inlineStr"/>
-      <c r="D180" t="inlineStr"/>
+      <c r="A180" t="inlineStr"/>
     </row>
     <row r="181">
-      <c r="A181" t="inlineStr">
-        <is>
-          <t>zipchain2_z_link_b_locking.stl</t>
-        </is>
-      </c>
-      <c r="B181" t="inlineStr"/>
-      <c r="C181" t="inlineStr"/>
-      <c r="D181" t="inlineStr"/>
+      <c r="A181" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Test_Prints</t>
+        </is>
+      </c>
     </row>
     <row r="182" ht="150" customHeight="1">
-      <c r="A182" t="inlineStr"/>
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Filament_Card.stl</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr"/>
+      <c r="C182" t="inlineStr"/>
+      <c r="D182" t="inlineStr"/>
     </row>
     <row r="183" ht="150" customHeight="1">
-      <c r="A183" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Test_Prints</t>
-        </is>
-      </c>
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Filament_Card_Caddy_25.stl</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr"/>
+      <c r="C183" t="inlineStr"/>
+      <c r="D183" t="inlineStr"/>
     </row>
     <row r="184" ht="150" customHeight="1">
       <c r="A184" t="inlineStr">
         <is>
-          <t>Filament_Card.stl</t>
+          <t>Heatset_Practice.stl</t>
         </is>
       </c>
       <c r="B184" t="inlineStr"/>
@@ -5759,7 +5781,7 @@
     <row r="185" ht="150" customHeight="1">
       <c r="A185" t="inlineStr">
         <is>
-          <t>Filament_Card_Caddy_25.stl</t>
+          <t>Voron_Design_Cube_v7.stl</t>
         </is>
       </c>
       <c r="B185" t="inlineStr"/>
@@ -5767,39 +5789,39 @@
       <c r="D185" t="inlineStr"/>
     </row>
     <row r="186">
-      <c r="A186" t="inlineStr">
-        <is>
-          <t>Heatset_Practice.stl</t>
-        </is>
-      </c>
-      <c r="B186" t="inlineStr"/>
-      <c r="C186" t="inlineStr"/>
-      <c r="D186" t="inlineStr"/>
+      <c r="A186" t="inlineStr"/>
     </row>
     <row r="187">
-      <c r="A187" t="inlineStr">
-        <is>
-          <t>Voron_Design_Cube_v7.stl</t>
-        </is>
-      </c>
-      <c r="B187" t="inlineStr"/>
-      <c r="C187" t="inlineStr"/>
-      <c r="D187" t="inlineStr"/>
+      <c r="A187" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Tools</t>
+        </is>
+      </c>
     </row>
     <row r="188" ht="150" customHeight="1">
-      <c r="A188" t="inlineStr"/>
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>bottom_panel_template.stl</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr"/>
+      <c r="C188" t="inlineStr"/>
+      <c r="D188" t="inlineStr"/>
     </row>
     <row r="189" ht="150" customHeight="1">
-      <c r="A189" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Tools</t>
-        </is>
-      </c>
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>MGN12_rail_guide_x2.stl</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr"/>
+      <c r="C189" t="inlineStr"/>
+      <c r="D189" t="inlineStr"/>
     </row>
     <row r="190" ht="150" customHeight="1">
       <c r="A190" t="inlineStr">
         <is>
-          <t>bottom_panel_template.stl</t>
+          <t>MGN9_rail_guide_x2.stl</t>
         </is>
       </c>
       <c r="B190" t="inlineStr"/>
@@ -5809,7 +5831,7 @@
     <row r="191" ht="150" customHeight="1">
       <c r="A191" t="inlineStr">
         <is>
-          <t>MGN12_rail_guide_x2.stl</t>
+          <t>pulley_jig.stl</t>
         </is>
       </c>
       <c r="B191" t="inlineStr"/>
@@ -5817,39 +5839,39 @@
       <c r="D191" t="inlineStr"/>
     </row>
     <row r="192">
-      <c r="A192" t="inlineStr">
-        <is>
-          <t>MGN9_rail_guide_x2.stl</t>
-        </is>
-      </c>
-      <c r="B192" t="inlineStr"/>
-      <c r="C192" t="inlineStr"/>
-      <c r="D192" t="inlineStr"/>
+      <c r="A192" t="inlineStr"/>
     </row>
     <row r="193">
-      <c r="A193" t="inlineStr">
-        <is>
-          <t>pulley_jig.stl</t>
-        </is>
-      </c>
-      <c r="B193" t="inlineStr"/>
-      <c r="C193" t="inlineStr"/>
-      <c r="D193" t="inlineStr"/>
+      <c r="A193" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Z_Drive</t>
+        </is>
+      </c>
     </row>
     <row r="194" ht="150" customHeight="1">
-      <c r="A194" t="inlineStr"/>
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>[a]_belt_tensioner_a_x2.stl</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr"/>
+      <c r="C194" t="inlineStr"/>
+      <c r="D194" t="inlineStr"/>
     </row>
     <row r="195" ht="150" customHeight="1">
-      <c r="A195" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Z_Drive</t>
-        </is>
-      </c>
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>[a]_belt_tensioner_b_x2.stl</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr"/>
+      <c r="C195" t="inlineStr"/>
+      <c r="D195" t="inlineStr"/>
     </row>
     <row r="196" ht="150" customHeight="1">
       <c r="A196" t="inlineStr">
         <is>
-          <t>[a]_belt_tensioner_a_x2.stl</t>
+          <t>[a]_z_drive_baseplate_a_x2.stl</t>
         </is>
       </c>
       <c r="B196" t="inlineStr"/>
@@ -5859,7 +5881,7 @@
     <row r="197" ht="150" customHeight="1">
       <c r="A197" t="inlineStr">
         <is>
-          <t>[a]_belt_tensioner_b_x2.stl</t>
+          <t>[a]_z_drive_baseplate_b_x2.stl</t>
         </is>
       </c>
       <c r="B197" t="inlineStr"/>
@@ -5869,7 +5891,7 @@
     <row r="198" ht="150" customHeight="1">
       <c r="A198" t="inlineStr">
         <is>
-          <t>[a]_z_drive_baseplate_a_x2.stl</t>
+          <t>z_drive_main_a_x2.stl</t>
         </is>
       </c>
       <c r="B198" t="inlineStr"/>
@@ -5879,7 +5901,7 @@
     <row r="199" ht="150" customHeight="1">
       <c r="A199" t="inlineStr">
         <is>
-          <t>[a]_z_drive_baseplate_b_x2.stl</t>
+          <t>z_drive_main_b_x2.stl</t>
         </is>
       </c>
       <c r="B199" t="inlineStr"/>
@@ -5889,7 +5911,7 @@
     <row r="200" ht="150" customHeight="1">
       <c r="A200" t="inlineStr">
         <is>
-          <t>z_drive_main_a_x2.stl</t>
+          <t>z_drive_retainer_a_x2.stl</t>
         </is>
       </c>
       <c r="B200" t="inlineStr"/>
@@ -5899,7 +5921,7 @@
     <row r="201" ht="150" customHeight="1">
       <c r="A201" t="inlineStr">
         <is>
-          <t>z_drive_main_b_x2.stl</t>
+          <t>z_drive_retainer_b_x2.stl</t>
         </is>
       </c>
       <c r="B201" t="inlineStr"/>
@@ -5909,7 +5931,7 @@
     <row r="202" ht="150" customHeight="1">
       <c r="A202" t="inlineStr">
         <is>
-          <t>z_drive_retainer_a_x2.stl</t>
+          <t>z_motor_mount_a_x2.stl</t>
         </is>
       </c>
       <c r="B202" t="inlineStr"/>
@@ -5919,7 +5941,7 @@
     <row r="203" ht="150" customHeight="1">
       <c r="A203" t="inlineStr">
         <is>
-          <t>z_drive_retainer_b_x2.stl</t>
+          <t>z_motor_mount_b_x2.stl</t>
         </is>
       </c>
       <c r="B203" t="inlineStr"/>
@@ -5927,84 +5949,64 @@
       <c r="D203" t="inlineStr"/>
     </row>
     <row r="204">
-      <c r="A204" t="inlineStr">
-        <is>
-          <t>z_motor_mount_a_x2.stl</t>
-        </is>
-      </c>
-      <c r="B204" t="inlineStr"/>
-      <c r="C204" t="inlineStr"/>
-      <c r="D204" t="inlineStr"/>
+      <c r="A204" t="inlineStr"/>
     </row>
     <row r="205">
-      <c r="A205" t="inlineStr">
-        <is>
-          <t>z_motor_mount_b_x2.stl</t>
-        </is>
-      </c>
-      <c r="B205" t="inlineStr"/>
-      <c r="C205" t="inlineStr"/>
-      <c r="D205" t="inlineStr"/>
+      <c r="A205" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Z_Endstop</t>
+        </is>
+      </c>
     </row>
     <row r="206" ht="150" customHeight="1">
-      <c r="A206" t="inlineStr"/>
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>nozzle_probe.stl</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr"/>
+      <c r="C206" t="inlineStr"/>
+      <c r="D206" t="inlineStr"/>
     </row>
     <row r="207">
-      <c r="A207" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Z_Endstop</t>
-        </is>
-      </c>
+      <c r="A207" t="inlineStr"/>
     </row>
     <row r="208">
-      <c r="A208" t="inlineStr">
-        <is>
-          <t>nozzle_probe.stl</t>
-        </is>
-      </c>
-      <c r="B208" t="inlineStr"/>
-      <c r="C208" t="inlineStr"/>
-      <c r="D208" t="inlineStr"/>
+      <c r="A208" s="1" t="inlineStr">
+        <is>
+          <t>Folder: Z_Idlers</t>
+        </is>
+      </c>
     </row>
     <row r="209" ht="150" customHeight="1">
-      <c r="A209" t="inlineStr"/>
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>[a]_z_tensioner_9mm_x4.stl</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr"/>
+      <c r="C209" t="inlineStr"/>
+      <c r="D209" t="inlineStr"/>
     </row>
     <row r="210" ht="150" customHeight="1">
-      <c r="A210" s="2" t="inlineStr">
-        <is>
-          <t>Folder: Z_Idlers</t>
-        </is>
-      </c>
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>z_tensioner_bracket_a_x2.stl</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr"/>
+      <c r="C210" t="inlineStr"/>
+      <c r="D210" t="inlineStr"/>
     </row>
     <row r="211" ht="150" customHeight="1">
       <c r="A211" t="inlineStr">
         <is>
-          <t>[a]_z_tensioner_9mm_x4.stl</t>
+          <t>z_tensioner_bracket_b_x2.stl</t>
         </is>
       </c>
       <c r="B211" t="inlineStr"/>
       <c r="C211" t="inlineStr"/>
       <c r="D211" t="inlineStr"/>
-    </row>
-    <row r="212">
-      <c r="A212" t="inlineStr">
-        <is>
-          <t>z_tensioner_bracket_a_x2.stl</t>
-        </is>
-      </c>
-      <c r="B212" t="inlineStr"/>
-      <c r="C212" t="inlineStr"/>
-      <c r="D212" t="inlineStr"/>
-    </row>
-    <row r="213">
-      <c r="A213" t="inlineStr">
-        <is>
-          <t>z_tensioner_bracket_b_x2.stl</t>
-        </is>
-      </c>
-      <c r="B213" t="inlineStr"/>
-      <c r="C213" t="inlineStr"/>
-      <c r="D213" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>